<commit_message>
set lower bound to variation in composition of Zooplankton to avoid having negative values
</commit_message>
<xml_diff>
--- a/output/article/Supp-mat_model_diets_10000.xlsx
+++ b/output/article/Supp-mat_model_diets_10000.xlsx
@@ -214,7 +214,7 @@
     <t xml:space="preserve">[Fere_att] L?pez-Su?rez et al 2012, O'Dwyer et al 2015, 
                                                             Elorriaga-Verplancken et al 2016, Zerbini &amp; Santos 1997,
                                                             Aguiar dos Santos &amp; Haimovici 2001, Donahue &amp; Perryman 2009, 
-                                                            Baird 2018, Sekiguchi et al 1992, [Glob_mel] Santos et al 2014, Spitz et al 2011, Santos et al 2014, Beaton et al 2007, Beaton et al 2009, Sekiguchi et al 1992, Beasley et al 2019, Gannon et al 1997</t>
+                                                            Baird 2018, Sekiguchi et al 1992, [Glob_mel] Santos et al 2014, Spitz et al 2011, Santos et al 2014, Beatson et al 2007, Beatson et al 2009, Sekiguchi et al 1992, Beasley et al 2019, Gannon et al 1997</t>
   </si>
   <si>
     <t xml:space="preserve">qualitative (Fere_att) &amp; quantitative (Glob_mel)</t>
@@ -239,7 +239,7 @@
     <t xml:space="preserve">Globicephala melas</t>
   </si>
   <si>
-    <t xml:space="preserve">Santos et al 2014, Spitz et al 2011, Santos et al 2014, Beaton et al 2007, Beaton et al 2009, Sekiguchi et al 1992, Beasley et al 2019, Gannon et al 1997</t>
+    <t xml:space="preserve">Santos et al 2014, Spitz et al 2011, Santos et al 2014, Beatson et al 2007, Beatson et al 2009, Sekiguchi et al 1992, Beasley et al 2019, Gannon et al 1997</t>
   </si>
   <si>
     <t xml:space="preserve">Gram_gri</t>
@@ -352,7 +352,7 @@
     <t xml:space="preserve">Watkins &amp; Schevill 1979, 
                               Witteven et al 2006, Filatova et al 2013,
                               Ryan et al 2014, Haro et al 2016,
-                              Fleming et al 2016, Claham 2018</t>
+                              Fleming et al 2016, Clapham 2018</t>
   </si>
   <si>
     <t xml:space="preserve">Orci_orc</t>
@@ -477,7 +477,7 @@
     <t xml:space="preserve">Stenella longirostris</t>
   </si>
   <si>
-    <t xml:space="preserve">[Sten_long] Silva et al 2004, Salum Soud 2010, 
+    <t xml:space="preserve">[Sten_long] Silva-Jr et al 2004, Salum Soud 2010, 
                                           Dolar et al 2003, Kiszka et al 2010, Clarke &amp; Young 1998, 
                                           Gross et al 2009, [Sten_att] Wang et al 2003</t>
   </si>
@@ -507,7 +507,7 @@
     <t xml:space="preserve">Sotalia guianensis</t>
   </si>
   <si>
-    <t xml:space="preserve">Daura-Jorge et al 2011, Pansard et al 2011, Rodrigues et al 2012</t>
+    <t xml:space="preserve">Daura-Jorge et al 2011, Pansard et al 2011, Rodrigues et al 2020</t>
   </si>
   <si>
     <t xml:space="preserve">Tursiops truncatus</t>

</xml_diff>